<commit_message>
Adição de tela inicial de configuração.
</commit_message>
<xml_diff>
--- a/perguntas_jeopardy.xlsx
+++ b/perguntas_jeopardy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1075293\Documents\Projeto_Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D8D217-3346-4D2C-8DD8-89D420C6E5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C1BD93-4119-4B9F-A69B-E8593847AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -785,7 +785,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Deixando "o que é" opcional
</commit_message>
<xml_diff>
--- a/perguntas_jeopardy.xlsx
+++ b/perguntas_jeopardy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1075293\Documents\Projeto_Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C1BD93-4119-4B9F-A69B-E8593847AFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5BF73-D6D0-4C74-A0B2-9D3D6327AEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,12 +190,6 @@
     <t>Levantamento de Requisitos</t>
   </si>
   <si>
-    <t>O que é um requisito funcional?</t>
-  </si>
-  <si>
-    <t>O que é a técnica de entrevista no levantamento de requisitos?</t>
-  </si>
-  <si>
     <t>Diferença entre organização visual e organização de dados.</t>
   </si>
   <si>
@@ -235,39 +229,21 @@
     <t>O que é uma interface que permite comunicação entre sistemas?</t>
   </si>
   <si>
-    <t>O que é uma API?</t>
-  </si>
-  <si>
     <t>O que é o sistema que registra alterações feitas no código?</t>
   </si>
   <si>
-    <t>O que é o controle de versão?</t>
-  </si>
-  <si>
     <t>Quais práticas garantem segurança no desenvolvimento back-end?</t>
   </si>
   <si>
-    <t>O que é a segurança no desenvolvimento back-end?</t>
-  </si>
-  <si>
     <t>O que é a parte visual de uma aplicação com a qual o usuário interage?</t>
   </si>
   <si>
-    <t>O que é o Front-End?</t>
-  </si>
-  <si>
     <t>O que é a linguagem que adiciona interatividade a páginas web?</t>
   </si>
   <si>
-    <t>O que é o JavaScript?</t>
-  </si>
-  <si>
     <t>O que é a capacidade de adaptação de páginas a diferentes dispositivos?</t>
   </si>
   <si>
-    <t>O que é responsividade em páginas web?</t>
-  </si>
-  <si>
     <t>Como a experiência do usuário (UX) influencia o desenvolvimento Front-End?</t>
   </si>
   <si>
@@ -280,9 +256,6 @@
     <t>O que é a conexão de dispositivos físicos à internet?</t>
   </si>
   <si>
-    <t>O que é Internet das Coisas (IoT)?</t>
-  </si>
-  <si>
     <t>O que é um dispositivo que detecta alterações físicas e gera dados?</t>
   </si>
   <si>
@@ -313,21 +286,12 @@
     <t>O que é a validação de uma unidade isolada do código?</t>
   </si>
   <si>
-    <t>O que é um teste unitário?</t>
-  </si>
-  <si>
     <t>O que é o teste realizado automaticamente por ferramentas?</t>
   </si>
   <si>
-    <t>O que é um teste automatizado?</t>
-  </si>
-  <si>
     <t>Como os testes contribuem para a qualidade de software?</t>
   </si>
   <si>
-    <t>O que é a importância dos testes para qualidade de software?</t>
-  </si>
-  <si>
     <t>O que é uma funcionalidade que o sistema deve executar?</t>
   </si>
   <si>
@@ -356,6 +320,42 @@
   </si>
   <si>
     <t>Qual protocolo de mensagens em IoT utiliza o modelo publish/subscribe?</t>
+  </si>
+  <si>
+    <t>O que é teste automatizado?</t>
+  </si>
+  <si>
+    <t>O que é teste unitário?</t>
+  </si>
+  <si>
+    <t>Qual é a importância dos testes para qualidade de software?</t>
+  </si>
+  <si>
+    <t>O que é responsividade?</t>
+  </si>
+  <si>
+    <t>O que é Front-End?</t>
+  </si>
+  <si>
+    <t>O que é JavaScript?</t>
+  </si>
+  <si>
+    <t>O que é segurança?</t>
+  </si>
+  <si>
+    <t>O que é controle de versão?</t>
+  </si>
+  <si>
+    <t>O que é API?</t>
+  </si>
+  <si>
+    <t>O que é cabeamento de rede?</t>
+  </si>
+  <si>
+    <t>O que é requisito funcional?</t>
+  </si>
+  <si>
+    <t>O que é a técnica de entrevista?</t>
   </si>
 </sst>
 </file>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,7 +818,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -832,10 +832,10 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -860,10 +860,10 @@
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -924,58 +924,58 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B13">
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -986,10 +986,10 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1000,10 +1000,10 @@
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1014,10 +1014,10 @@
         <v>150</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1028,10 +1028,10 @@
         <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,10 +1070,10 @@
         <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1154,10 +1154,10 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1168,10 +1168,10 @@
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1182,10 +1182,10 @@
         <v>150</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -1196,10 +1196,10 @@
         <v>200</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -1210,10 +1210,10 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -1224,10 +1224,10 @@
         <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -1238,10 +1238,10 @@
         <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1252,10 +1252,10 @@
         <v>200</v>
       </c>
       <c r="C33" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -1378,7 +1378,7 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
         <v>50</v>
@@ -1392,7 +1392,7 @@
         <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
         <v>51</v>
@@ -1406,10 +1406,10 @@
         <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1420,66 +1420,66 @@
         <v>200</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B46">
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B47">
         <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B48">
         <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B49">
         <v>200</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>